<commit_message>
report commesse e collaboratori - miglioramento interfaccia
</commit_message>
<xml_diff>
--- a/static/report_commessa.xlsx
+++ b/static/report_commessa.xlsx
@@ -187,7 +187,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -207,6 +207,10 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="1" t="n">
+        <f aca="false">SUM(F12:F500)</f>
+        <v>0</v>
+      </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -215,6 +219,10 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">SUM(C12:C500)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>